<commit_message>
dateINput invalid class eklemesi
</commit_message>
<xml_diff>
--- a/resource/dateInput.xlsx
+++ b/resource/dateInput.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
   <si>
     <t>R1</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Boundary Values</t>
   </si>
   <si>
-    <t>ECs and Values</t>
-  </si>
-  <si>
     <t>{month | month has 30 days}</t>
   </si>
   <si>
@@ -223,24 +220,6 @@
     <t>{year | 1812 ≤ year ≤ 2012 AND 0 ≠ year mod 4}</t>
   </si>
   <si>
-    <t>april</t>
-  </si>
-  <si>
-    <t>january</t>
-  </si>
-  <si>
-    <t>february</t>
-  </si>
-  <si>
-    <t>june</t>
-  </si>
-  <si>
-    <t>december</t>
-  </si>
-  <si>
-    <t>november</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
@@ -248,6 +227,87 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>Valid ECs and Values</t>
+  </si>
+  <si>
+    <t>Invalid ECs and Values</t>
+  </si>
+  <si>
+    <t>Invalid Classes</t>
+  </si>
+  <si>
+    <t>{month | month &lt; 1}</t>
+  </si>
+  <si>
+    <t>{month | month &gt; 12}</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>{day | day &lt; 1}</t>
+  </si>
+  <si>
+    <t>{day | day &gt; 31}</t>
+  </si>
+  <si>
+    <t>{year | year &lt; 1812}</t>
+  </si>
+  <si>
+    <t>{year | year &gt; 2012}</t>
+  </si>
+  <si>
+    <t>Valid Classes</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -443,17 +503,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -470,6 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bağlı Hücre" xfId="1" builtinId="24"/>
@@ -842,10 +902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,332 +920,451 @@
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="12" t="s">
+      <c r="D1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="13"/>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D3" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="22">
+        <v>12</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21">
         <v>15</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="21">
         <v>29</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="21">
         <v>30</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="21">
         <v>31</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="8">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="22">
         <v>0</v>
       </c>
-      <c r="O4" s="8">
+      <c r="U4" s="22">
         <v>1</v>
       </c>
-      <c r="P4" s="8">
+      <c r="V4" s="22">
         <v>2</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="W4" s="22">
         <v>15</v>
       </c>
-      <c r="R4" s="8">
+      <c r="X4" s="22">
         <v>30</v>
       </c>
-      <c r="S4" s="8">
+      <c r="Y4" s="22">
         <v>31</v>
       </c>
-      <c r="T4" s="8">
+      <c r="Z4" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21">
         <v>1900</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="21">
         <v>1996</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="21">
         <v>1997</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="T5" s="22">
         <v>1811</v>
       </c>
-      <c r="O5" s="8">
+      <c r="U5" s="22">
         <v>1812</v>
       </c>
-      <c r="P5" s="8">
+      <c r="V5" s="22">
         <v>1813</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="W5" s="22">
         <v>1912</v>
       </c>
-      <c r="R5" s="8">
+      <c r="X5" s="22">
         <v>2011</v>
       </c>
-      <c r="S5" s="8">
+      <c r="Y5" s="22">
         <v>2012</v>
       </c>
-      <c r="T5" s="8">
+      <c r="Z5" s="22">
         <v>2013</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>62</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>